<commit_message>
Stop building Fig. 3
</commit_message>
<xml_diff>
--- a/manuscript/Author Checklist - EMBO J.xlsx
+++ b/manuscript/Author Checklist - EMBO J.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10323"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/asm/Downloads/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrillus/Dropbox/Meyer/systemsSerology/manuscript/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1732F48B-5FE7-E643-B450-449C49DF96E7}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEBFC33-E010-F041-B20D-9426B6A173CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="1260" windowWidth="27120" windowHeight="29800" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="9240" yWindow="500" windowWidth="33500" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="128" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
   <si>
     <t>PLEASE NOTE THAT THIS CHECKLIST WILL BE PUBLISHED ALONGSIDE YOUR PAPER</t>
   </si>
@@ -717,16 +717,19 @@
     <t>Reporting Checklist For Life Sciences Articles (Rev. June 2017)</t>
   </si>
   <si>
-    <t xml:space="preserve">Manuscript Number: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Journal Submitted to: </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Corresponding Author Name: </t>
-  </si>
-  <si>
     <t>No.</t>
+  </si>
+  <si>
+    <t>Corresponding Author Name: Aaron S. Meyer</t>
+  </si>
+  <si>
+    <t>Journal Submitted to: Molecular Systems Biology</t>
+  </si>
+  <si>
+    <t>Manuscript Number: MSB-2021-10243</t>
+  </si>
+  <si>
+    <t>n/a</t>
   </si>
 </sst>
 </file>
@@ -1119,6 +1122,57 @@
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1127,14 +1181,14 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
@@ -1145,61 +1199,10 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -1547,8 +1550,8 @@
   </sheetPr>
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A78" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E91" sqref="E91"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E83" sqref="E83:F83"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1569,60 +1572,60 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:7" ht="37" x14ac:dyDescent="0.45">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="35" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
+      <c r="C2" s="36"/>
+      <c r="D2" s="36"/>
       <c r="E2" s="6"/>
     </row>
     <row r="4" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B4" s="40" t="s">
+      <c r="B4" s="59" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="41"/>
-      <c r="D4" s="41"/>
+      <c r="C4" s="60"/>
+      <c r="D4" s="60"/>
       <c r="E4" s="22"/>
       <c r="F4" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B5" s="61" t="s">
+      <c r="B5" s="41" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="62"/>
-      <c r="D5" s="62"/>
+      <c r="C5" s="42"/>
+      <c r="D5" s="42"/>
       <c r="E5" s="22"/>
       <c r="F5" s="26"/>
     </row>
     <row r="6" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="56" t="s">
-        <v>109</v>
-      </c>
-      <c r="C7" s="63"/>
-      <c r="D7" s="64"/>
+      <c r="B7" s="43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C7" s="44"/>
+      <c r="D7" s="45"/>
       <c r="E7" s="23"/>
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="56" t="s">
-        <v>108</v>
-      </c>
-      <c r="C8" s="63"/>
-      <c r="D8" s="64"/>
+      <c r="B8" s="43" t="s">
+        <v>109</v>
+      </c>
+      <c r="C8" s="44"/>
+      <c r="D8" s="45"/>
       <c r="E8" s="23"/>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="56" t="s">
-        <v>107</v>
-      </c>
-      <c r="C9" s="57"/>
-      <c r="D9" s="58"/>
+      <c r="B9" s="43" t="s">
+        <v>110</v>
+      </c>
+      <c r="C9" s="62"/>
+      <c r="D9" s="63"/>
       <c r="E9" s="23"/>
       <c r="F9" s="28" t="s">
         <v>41</v>
@@ -1640,11 +1643,11 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B11" s="43" t="s">
+      <c r="B11" s="37" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="43"/>
-      <c r="D11" s="44"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="38"/>
       <c r="E11" s="17"/>
       <c r="F11" s="28" t="s">
         <v>39</v>
@@ -1654,11 +1657,11 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="76" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="51" t="s">
+      <c r="B12" s="39" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="51"/>
-      <c r="D12" s="52"/>
+      <c r="C12" s="39"/>
+      <c r="D12" s="40"/>
       <c r="E12" s="18"/>
       <c r="F12" s="28" t="s">
         <v>46</v>
@@ -1676,11 +1679,11 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B14" s="43" t="s">
+      <c r="B14" s="37" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="43"/>
-      <c r="D14" s="44"/>
+      <c r="C14" s="37"/>
+      <c r="D14" s="38"/>
       <c r="E14" s="17"/>
       <c r="F14" s="29" t="s">
         <v>50</v>
@@ -1690,11 +1693,11 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B15" s="43" t="s">
+      <c r="B15" s="37" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="43"/>
-      <c r="D15" s="44"/>
+      <c r="C15" s="37"/>
+      <c r="D15" s="38"/>
       <c r="E15" s="17"/>
       <c r="F15" s="29" t="s">
         <v>52</v>
@@ -1704,11 +1707,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B16" s="43" t="s">
+      <c r="B16" s="37" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="43"/>
-      <c r="D16" s="44"/>
+      <c r="C16" s="37"/>
+      <c r="D16" s="38"/>
       <c r="E16" s="17"/>
       <c r="F16" s="29" t="s">
         <v>54</v>
@@ -1721,10 +1724,10 @@
       <c r="B17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="45" t="s">
+      <c r="C17" s="48" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="46"/>
+      <c r="D17" s="55"/>
       <c r="E17" s="24"/>
       <c r="F17" s="29" t="s">
         <v>56</v>
@@ -1737,10 +1740,10 @@
       <c r="B18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="45" t="s">
+      <c r="C18" s="48" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="46"/>
+      <c r="D18" s="55"/>
       <c r="E18" s="24"/>
       <c r="F18" s="28" t="s">
         <v>58</v>
@@ -1753,10 +1756,10 @@
       <c r="B19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="45" t="s">
+      <c r="C19" s="48" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="46"/>
+      <c r="D19" s="55"/>
       <c r="E19" s="24"/>
       <c r="F19" s="28" t="s">
         <v>61</v>
@@ -1769,10 +1772,10 @@
       <c r="B20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="45" t="s">
+      <c r="C20" s="48" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="46"/>
+      <c r="D20" s="55"/>
       <c r="E20" s="24"/>
       <c r="F20" s="28" t="s">
         <v>12</v>
@@ -1785,10 +1788,10 @@
       <c r="B21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="45" t="s">
+      <c r="C21" s="48" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="46"/>
+      <c r="D21" s="55"/>
       <c r="E21" s="24"/>
       <c r="F21" s="28" t="s">
         <v>14</v>
@@ -1805,11 +1808,11 @@
     </row>
     <row r="23" spans="1:17" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="43" t="s">
+      <c r="B23" s="37" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="43"/>
-      <c r="D23" s="44"/>
+      <c r="C23" s="37"/>
+      <c r="D23" s="38"/>
       <c r="E23" s="17"/>
       <c r="F23" s="28" t="s">
         <v>18</v>
@@ -1830,11 +1833,11 @@
     </row>
     <row r="24" spans="1:17" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
-      <c r="B24" s="43" t="s">
+      <c r="B24" s="37" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="43"/>
-      <c r="D24" s="48"/>
+      <c r="C24" s="37"/>
+      <c r="D24" s="56"/>
       <c r="E24" s="19"/>
       <c r="F24" s="28" t="s">
         <v>16</v>
@@ -1857,10 +1860,10 @@
       <c r="B25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="45" t="s">
+      <c r="C25" s="48" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="47"/>
+      <c r="D25" s="49"/>
       <c r="E25" s="25"/>
       <c r="F25" s="28" t="s">
         <v>25</v>
@@ -1873,10 +1876,10 @@
       <c r="B26" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="45" t="s">
+      <c r="C26" s="48" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="47"/>
+      <c r="D26" s="49"/>
       <c r="E26" s="25"/>
       <c r="F26" s="28" t="s">
         <v>21</v>
@@ -1889,10 +1892,10 @@
       <c r="B27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="45" t="s">
+      <c r="C27" s="48" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="47"/>
+      <c r="D27" s="49"/>
       <c r="E27" s="25"/>
       <c r="F27" s="28" t="s">
         <v>23</v>
@@ -1905,50 +1908,50 @@
       <c r="B28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="45" t="s">
+      <c r="C28" s="48" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="47"/>
+      <c r="D28" s="49"/>
       <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="45" t="s">
+      <c r="C29" s="48" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="47"/>
+      <c r="D29" s="49"/>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:17" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="45" t="s">
+      <c r="C30" s="48" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="47"/>
+      <c r="D30" s="49"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="45" t="s">
+      <c r="C31" s="48" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="47"/>
+      <c r="D31" s="49"/>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="45" t="s">
+      <c r="C32" s="48" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="47"/>
+      <c r="D32" s="49"/>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:7" ht="66" x14ac:dyDescent="0.25">
@@ -2018,38 +2021,38 @@
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="51" t="s">
+      <c r="B40" s="39" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="51"/>
-      <c r="D40" s="52"/>
+      <c r="C40" s="39"/>
+      <c r="D40" s="40"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="2:7" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="53" t="s">
+      <c r="B41" s="50" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="53"/>
-      <c r="D41" s="54"/>
+      <c r="C41" s="50"/>
+      <c r="D41" s="51"/>
       <c r="E41" s="20"/>
     </row>
     <row r="43" spans="2:7" ht="95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="55" t="s">
+      <c r="B43" s="52" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="55"/>
-      <c r="D43" s="55"/>
+      <c r="C43" s="52"/>
+      <c r="D43" s="52"/>
     </row>
     <row r="45" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B45" s="38" t="s">
+      <c r="B45" s="46" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="38"/>
-      <c r="D45" s="39"/>
-      <c r="E45" s="49" t="s">
+      <c r="C45" s="46"/>
+      <c r="D45" s="47"/>
+      <c r="E45" s="57" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="50"/>
+      <c r="F45" s="58"/>
       <c r="G45" s="27"/>
     </row>
     <row r="46" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2057,85 +2060,85 @@
       <c r="D47" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="42"/>
-      <c r="F47" s="36"/>
+      <c r="E47" s="61"/>
+      <c r="F47" s="54"/>
     </row>
     <row r="48" spans="2:7" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="42"/>
-      <c r="F48" s="36"/>
+      <c r="E48" s="61"/>
+      <c r="F48" s="54"/>
     </row>
     <row r="49" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="35"/>
-      <c r="F49" s="36"/>
+      <c r="E49" s="53"/>
+      <c r="F49" s="54"/>
     </row>
     <row r="50" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="35"/>
-      <c r="F50" s="36"/>
+      <c r="E50" s="53"/>
+      <c r="F50" s="54"/>
     </row>
     <row r="51" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="35"/>
-      <c r="F51" s="36"/>
+      <c r="E51" s="53"/>
+      <c r="F51" s="54"/>
     </row>
     <row r="52" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="35"/>
-      <c r="F52" s="36"/>
+      <c r="E52" s="53"/>
+      <c r="F52" s="54"/>
     </row>
     <row r="53" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="35"/>
-      <c r="F53" s="36"/>
+      <c r="E53" s="53"/>
+      <c r="F53" s="54"/>
     </row>
     <row r="54" spans="2:6" ht="131" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="35"/>
-      <c r="F54" s="36"/>
+      <c r="E54" s="53"/>
+      <c r="F54" s="54"/>
     </row>
     <row r="55" spans="2:6" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E55" s="35"/>
-      <c r="F55" s="36"/>
+      <c r="E55" s="53"/>
+      <c r="F55" s="54"/>
     </row>
     <row r="56" spans="2:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="35"/>
-      <c r="F56" s="37"/>
+      <c r="E56" s="53"/>
+      <c r="F56" s="64"/>
     </row>
     <row r="57" spans="2:6" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E57" s="35"/>
-      <c r="F57" s="36"/>
+      <c r="E57" s="53"/>
+      <c r="F57" s="54"/>
     </row>
     <row r="59" spans="2:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="B59" s="38" t="s">
+      <c r="B59" s="46" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="38"/>
-      <c r="D59" s="39"/>
+      <c r="C59" s="46"/>
+      <c r="D59" s="47"/>
       <c r="E59" s="21"/>
     </row>
     <row r="60" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2143,15 +2146,15 @@
       <c r="D61" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
+      <c r="E61" s="53"/>
+      <c r="F61" s="54"/>
     </row>
     <row r="62" spans="2:6" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="35"/>
-      <c r="F62" s="36"/>
+      <c r="E62" s="53"/>
+      <c r="F62" s="54"/>
     </row>
     <row r="63" spans="2:6" ht="22" x14ac:dyDescent="0.25">
       <c r="D63" s="13" t="s">
@@ -2166,11 +2169,11 @@
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B65" s="38" t="s">
+      <c r="B65" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="38"/>
-      <c r="D65" s="39"/>
+      <c r="C65" s="46"/>
+      <c r="D65" s="47"/>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2178,35 +2181,41 @@
       <c r="D67" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="35"/>
-      <c r="F67" s="36"/>
+      <c r="E67" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F67" s="54"/>
       <c r="H67" s="16"/>
     </row>
     <row r="68" spans="2:8" ht="113" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E68" s="35"/>
-      <c r="F68" s="36"/>
+      <c r="E68" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F68" s="54"/>
       <c r="H68" s="16"/>
     </row>
     <row r="69" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="35"/>
-      <c r="F69" s="36"/>
+      <c r="E69" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F69" s="54"/>
       <c r="H69" s="16"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H70" s="16"/>
     </row>
     <row r="71" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B71" s="38" t="s">
+      <c r="B71" s="46" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="38"/>
-      <c r="D71" s="39"/>
+      <c r="C71" s="46"/>
+      <c r="D71" s="47"/>
       <c r="E71" s="21"/>
     </row>
     <row r="72" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2214,61 +2223,75 @@
       <c r="D73" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="35"/>
-      <c r="F73" s="36"/>
+      <c r="E73" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F73" s="54"/>
     </row>
     <row r="74" spans="2:8" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E74" s="35"/>
-      <c r="F74" s="36"/>
+      <c r="E74" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F74" s="54"/>
       <c r="H74" s="16"/>
     </row>
     <row r="75" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="35"/>
-      <c r="F75" s="36"/>
+      <c r="E75" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F75" s="54"/>
       <c r="H75" s="16"/>
     </row>
     <row r="76" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E76" s="35"/>
-      <c r="F76" s="36"/>
+      <c r="E76" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F76" s="54"/>
       <c r="H76" s="16"/>
     </row>
     <row r="77" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E77" s="35"/>
-      <c r="F77" s="36"/>
+      <c r="E77" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F77" s="54"/>
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="35"/>
-      <c r="F78" s="36"/>
+      <c r="E78" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F78" s="54"/>
     </row>
     <row r="79" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E79" s="35"/>
-      <c r="F79" s="36"/>
+      <c r="E79" s="53" t="s">
+        <v>111</v>
+      </c>
+      <c r="F79" s="54"/>
     </row>
     <row r="81" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B81" s="38" t="s">
+      <c r="B81" s="46" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="38"/>
-      <c r="D81" s="39"/>
+      <c r="C81" s="46"/>
+      <c r="D81" s="47"/>
       <c r="E81" s="21"/>
     </row>
     <row r="82" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2276,31 +2299,31 @@
       <c r="D83" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="35"/>
-      <c r="F83" s="36"/>
+      <c r="E83" s="53"/>
+      <c r="F83" s="54"/>
     </row>
     <row r="84" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E84" s="35"/>
-      <c r="F84" s="36"/>
+      <c r="E84" s="53"/>
+      <c r="F84" s="54"/>
       <c r="H84" s="16"/>
     </row>
     <row r="85" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="35"/>
-      <c r="F85" s="36"/>
+      <c r="E85" s="53"/>
+      <c r="F85" s="54"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="2:8" ht="133" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E86" s="35"/>
-      <c r="F86" s="36"/>
+      <c r="E86" s="53"/>
+      <c r="F86" s="54"/>
       <c r="H86" s="16"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2309,11 +2332,11 @@
       <c r="F87" s="14"/>
     </row>
     <row r="88" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B88" s="38" t="s">
+      <c r="B88" s="46" t="s">
         <v>38</v>
       </c>
-      <c r="C88" s="38"/>
-      <c r="D88" s="39"/>
+      <c r="C88" s="46"/>
+      <c r="D88" s="47"/>
       <c r="E88" s="21"/>
       <c r="H88" s="16"/>
     </row>
@@ -2324,10 +2347,10 @@
       <c r="D90" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E90" s="35" t="s">
-        <v>110</v>
-      </c>
-      <c r="F90" s="36"/>
+      <c r="E90" s="53" t="s">
+        <v>107</v>
+      </c>
+      <c r="F90" s="54"/>
       <c r="H90" s="16"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -2342,26 +2365,33 @@
   </sheetData>
   <sheetProtection password="DCD2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="64">
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E48:F48"/>
+    <mergeCell ref="E49:F49"/>
+    <mergeCell ref="E50:F50"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="E62:F62"/>
+    <mergeCell ref="E54:F54"/>
+    <mergeCell ref="E55:F55"/>
+    <mergeCell ref="E56:F56"/>
+    <mergeCell ref="E57:F57"/>
+    <mergeCell ref="E61:F61"/>
     <mergeCell ref="E51:F51"/>
     <mergeCell ref="E52:F52"/>
     <mergeCell ref="E53:F53"/>
@@ -2377,35 +2407,28 @@
     <mergeCell ref="C21:D21"/>
     <mergeCell ref="E45:F45"/>
     <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
     <mergeCell ref="B4:D4"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="E48:F48"/>
-    <mergeCell ref="E49:F49"/>
-    <mergeCell ref="E50:F50"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="E62:F62"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="E54:F54"/>
-    <mergeCell ref="E55:F55"/>
-    <mergeCell ref="E56:F56"/>
-    <mergeCell ref="E57:F57"/>
-    <mergeCell ref="E61:F61"/>
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E75:F75"/>
-    <mergeCell ref="E86:F86"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Update Author Checklist - EMBO J.xlsx
</commit_message>
<xml_diff>
--- a/manuscript/Author Checklist - EMBO J.xlsx
+++ b/manuscript/Author Checklist - EMBO J.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrillus/Dropbox/Meyer/systemsSerology/manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEBFC33-E010-F041-B20D-9426B6A173CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892F7B31-12C9-6F41-A575-0E3C067CAE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="500" windowWidth="33500" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>PLEASE NOTE THAT THIS CHECKLIST WILL BE PUBLISHED ALONGSIDE YOUR PAPER</t>
   </si>
@@ -717,19 +717,46 @@
     <t>Reporting Checklist For Life Sciences Articles (Rev. June 2017)</t>
   </si>
   <si>
+    <t>Corresponding Author Name:  Aaron Meyer</t>
+  </si>
+  <si>
+    <t>N/A: No animals were used.</t>
+  </si>
+  <si>
+    <t>N/A: No human subjects were used.</t>
+  </si>
+  <si>
+    <t>See above: We will deposit our data.</t>
+  </si>
+  <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Corresponding Author Name: Aaron S. Meyer</t>
-  </si>
-  <si>
-    <t>Journal Submitted to: Molecular Systems Biology</t>
+    <t>Journal Submitted to:  Molecular Systems Biology</t>
   </si>
   <si>
     <t>Manuscript Number: MSB-2021-10243</t>
   </si>
   <si>
-    <t>n/a</t>
+    <t>N/A: No cell lines were used.</t>
+  </si>
+  <si>
+    <t>N/A: No antibody measurements were performed.</t>
+  </si>
+  <si>
+    <t>N/A: We don't have any hypothesis testing.</t>
+  </si>
+  <si>
+    <t>N/A: Not an animal study.</t>
+  </si>
+  <si>
+    <t>N/A: Samples were computationally randomized.</t>
+  </si>
+  <si>
+    <t>N/A: This is an analysis of existing data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HIV-1 viral control data comes from a previous study (Alter et al, 2018). All analysis was implemented in Python v3.9 and can be found at https://github.com/meyer-lab/systemsSerology.  We have provided a "Data Availability" section at the end of our paper. We will also generate a Digital Object Identifier (DOI) for our code once the code is finalized for the paper. </t>
   </si>
 </sst>
 </file>
@@ -1122,57 +1149,6 @@
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1181,22 +1157,16 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1204,6 +1174,63 @@
     <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1550,8 +1577,8 @@
   </sheetPr>
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:F83"/>
+    <sheetView tabSelected="1" topLeftCell="B79" zoomScale="110" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85:F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1572,60 +1599,60 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:7" ht="37" x14ac:dyDescent="0.45">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="6"/>
     </row>
     <row r="4" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="22"/>
       <c r="F4" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="22"/>
       <c r="F5" s="26"/>
     </row>
     <row r="6" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
+      <c r="B7" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="23"/>
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="B8" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="23"/>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
+      <c r="B9" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="23"/>
       <c r="F9" s="28" t="s">
         <v>41</v>
@@ -1643,11 +1670,11 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="17"/>
       <c r="F11" s="28" t="s">
         <v>39</v>
@@ -1657,11 +1684,11 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="76" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="18"/>
       <c r="F12" s="28" t="s">
         <v>46</v>
@@ -1679,11 +1706,11 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="17"/>
       <c r="F14" s="29" t="s">
         <v>50</v>
@@ -1693,11 +1720,11 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="17"/>
       <c r="F15" s="29" t="s">
         <v>52</v>
@@ -1707,11 +1734,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="17"/>
       <c r="F16" s="29" t="s">
         <v>54</v>
@@ -1724,10 +1751,10 @@
       <c r="B17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="24"/>
       <c r="F17" s="29" t="s">
         <v>56</v>
@@ -1740,10 +1767,10 @@
       <c r="B18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="24"/>
       <c r="F18" s="28" t="s">
         <v>58</v>
@@ -1756,10 +1783,10 @@
       <c r="B19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="24"/>
       <c r="F19" s="28" t="s">
         <v>61</v>
@@ -1772,10 +1799,10 @@
       <c r="B20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="55"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="24"/>
       <c r="F20" s="28" t="s">
         <v>12</v>
@@ -1788,10 +1815,10 @@
       <c r="B21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="55"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="24"/>
       <c r="F21" s="28" t="s">
         <v>14</v>
@@ -1808,11 +1835,11 @@
     </row>
     <row r="23" spans="1:17" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="17"/>
       <c r="F23" s="28" t="s">
         <v>18</v>
@@ -1833,11 +1860,11 @@
     </row>
     <row r="24" spans="1:17" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="56"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="19"/>
       <c r="F24" s="28" t="s">
         <v>16</v>
@@ -1860,10 +1887,10 @@
       <c r="B25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="25"/>
       <c r="F25" s="28" t="s">
         <v>25</v>
@@ -1876,10 +1903,10 @@
       <c r="B26" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="49"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="25"/>
       <c r="F26" s="28" t="s">
         <v>21</v>
@@ -1892,10 +1919,10 @@
       <c r="B27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="49"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="25"/>
       <c r="F27" s="28" t="s">
         <v>23</v>
@@ -1908,50 +1935,50 @@
       <c r="B28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="49"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:17" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="49"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="49"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="49"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:7" ht="66" x14ac:dyDescent="0.25">
@@ -2021,38 +2048,38 @@
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="2:7" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="51"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="20"/>
     </row>
     <row r="43" spans="2:7" ht="95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
     </row>
     <row r="45" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="57" t="s">
+      <c r="C45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="58"/>
+      <c r="F45" s="51"/>
       <c r="G45" s="27"/>
     </row>
     <row r="46" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2060,85 +2087,107 @@
       <c r="D47" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="61"/>
-      <c r="F47" s="54"/>
+      <c r="E47" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="36"/>
     </row>
     <row r="48" spans="2:7" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="61"/>
-      <c r="F48" s="54"/>
+      <c r="E48" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="36"/>
     </row>
     <row r="49" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="53"/>
-      <c r="F49" s="54"/>
+      <c r="E49" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="54"/>
+      <c r="E50" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="53"/>
-      <c r="F51" s="54"/>
+      <c r="E51" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" s="36"/>
     </row>
     <row r="52" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="53"/>
-      <c r="F52" s="54"/>
+      <c r="E52" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" s="36"/>
     </row>
     <row r="53" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="53"/>
-      <c r="F53" s="54"/>
+      <c r="E53" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" s="36"/>
     </row>
     <row r="54" spans="2:6" ht="131" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="53"/>
-      <c r="F54" s="54"/>
+      <c r="E54" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" s="36"/>
     </row>
     <row r="55" spans="2:6" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E55" s="53"/>
-      <c r="F55" s="54"/>
+      <c r="E55" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="2:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="64"/>
+      <c r="E56" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="43"/>
     </row>
     <row r="57" spans="2:6" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E57" s="53"/>
-      <c r="F57" s="54"/>
+      <c r="E57" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="36"/>
     </row>
     <row r="59" spans="2:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="46"/>
-      <c r="D59" s="47"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
       <c r="E59" s="21"/>
     </row>
     <row r="60" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2146,15 +2195,19 @@
       <c r="D61" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="53"/>
-      <c r="F61" s="54"/>
+      <c r="E61" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="36"/>
     </row>
     <row r="62" spans="2:6" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="53"/>
-      <c r="F62" s="54"/>
+      <c r="E62" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F62" s="36"/>
     </row>
     <row r="63" spans="2:6" ht="22" x14ac:dyDescent="0.25">
       <c r="D63" s="13" t="s">
@@ -2169,11 +2222,11 @@
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="46"/>
-      <c r="D65" s="47"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="38"/>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2181,41 +2234,41 @@
       <c r="D67" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F67" s="54"/>
+      <c r="E67" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67" s="36"/>
       <c r="H67" s="16"/>
     </row>
     <row r="68" spans="2:8" ht="113" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E68" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F68" s="54"/>
+      <c r="E68" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="36"/>
       <c r="H68" s="16"/>
     </row>
     <row r="69" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F69" s="54"/>
+      <c r="E69" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" s="36"/>
       <c r="H69" s="16"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H70" s="16"/>
     </row>
     <row r="71" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="46"/>
-      <c r="D71" s="47"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="38"/>
       <c r="E71" s="21"/>
     </row>
     <row r="72" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2223,75 +2276,75 @@
       <c r="D73" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F73" s="54"/>
+      <c r="E73" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F73" s="36"/>
     </row>
     <row r="74" spans="2:8" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E74" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F74" s="54"/>
+      <c r="E74" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F74" s="36"/>
       <c r="H74" s="16"/>
     </row>
     <row r="75" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F75" s="54"/>
+      <c r="E75" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" s="36"/>
       <c r="H75" s="16"/>
     </row>
     <row r="76" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E76" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F76" s="54"/>
+      <c r="E76" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="36"/>
       <c r="H76" s="16"/>
     </row>
     <row r="77" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E77" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F77" s="54"/>
+      <c r="E77" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="36"/>
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F78" s="54"/>
+      <c r="E78" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" s="36"/>
     </row>
     <row r="79" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E79" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F79" s="54"/>
+      <c r="E79" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="36"/>
     </row>
     <row r="81" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B81" s="46" t="s">
+      <c r="B81" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="46"/>
-      <c r="D81" s="47"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="38"/>
       <c r="E81" s="21"/>
     </row>
     <row r="82" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2299,31 +2352,39 @@
       <c r="D83" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="53"/>
-      <c r="F83" s="54"/>
+      <c r="E83" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F83" s="36"/>
     </row>
     <row r="84" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E84" s="53"/>
-      <c r="F84" s="54"/>
+      <c r="E84" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84" s="36"/>
       <c r="H84" s="16"/>
     </row>
     <row r="85" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="53"/>
-      <c r="F85" s="54"/>
+      <c r="E85" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85" s="36"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="2:8" ht="133" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E86" s="53"/>
-      <c r="F86" s="54"/>
+      <c r="E86" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86" s="36"/>
       <c r="H86" s="16"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2332,11 +2393,11 @@
       <c r="F87" s="14"/>
     </row>
     <row r="88" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B88" s="46" t="s">
+      <c r="B88" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C88" s="46"/>
-      <c r="D88" s="47"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="38"/>
       <c r="E88" s="21"/>
       <c r="H88" s="16"/>
     </row>
@@ -2347,10 +2408,10 @@
       <c r="D90" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E90" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="F90" s="54"/>
+      <c r="E90" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="36"/>
       <c r="H90" s="16"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -2365,23 +2426,37 @@
   </sheetData>
   <sheetProtection password="DCD2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="64">
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
@@ -2398,37 +2473,23 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Update Author Checklist - EMBO J.xlsx (#327)
</commit_message>
<xml_diff>
--- a/manuscript/Author Checklist - EMBO J.xlsx
+++ b/manuscript/Author Checklist - EMBO J.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10613"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cyrillus/Dropbox/Meyer/systemsSerology/manuscript/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/hakan/Downloads/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DEBFC33-E010-F041-B20D-9426B6A173CE}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{892F7B31-12C9-6F41-A575-0E3C067CAE89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9240" yWindow="500" windowWidth="33500" windowHeight="26600" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="33600" windowHeight="19860" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="155" uniqueCount="121">
   <si>
     <t>PLEASE NOTE THAT THIS CHECKLIST WILL BE PUBLISHED ALONGSIDE YOUR PAPER</t>
   </si>
@@ -717,19 +717,46 @@
     <t>Reporting Checklist For Life Sciences Articles (Rev. June 2017)</t>
   </si>
   <si>
+    <t>Corresponding Author Name:  Aaron Meyer</t>
+  </si>
+  <si>
+    <t>N/A: No animals were used.</t>
+  </si>
+  <si>
+    <t>N/A: No human subjects were used.</t>
+  </si>
+  <si>
+    <t>See above: We will deposit our data.</t>
+  </si>
+  <si>
     <t>No.</t>
   </si>
   <si>
-    <t>Corresponding Author Name: Aaron S. Meyer</t>
-  </si>
-  <si>
-    <t>Journal Submitted to: Molecular Systems Biology</t>
+    <t>Journal Submitted to:  Molecular Systems Biology</t>
   </si>
   <si>
     <t>Manuscript Number: MSB-2021-10243</t>
   </si>
   <si>
-    <t>n/a</t>
+    <t>N/A: No cell lines were used.</t>
+  </si>
+  <si>
+    <t>N/A: No antibody measurements were performed.</t>
+  </si>
+  <si>
+    <t>N/A: We don't have any hypothesis testing.</t>
+  </si>
+  <si>
+    <t>N/A: Not an animal study.</t>
+  </si>
+  <si>
+    <t>N/A: Samples were computationally randomized.</t>
+  </si>
+  <si>
+    <t>N/A: This is an analysis of existing data.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">The HIV-1 viral control data comes from a previous study (Alter et al, 2018). All analysis was implemented in Python v3.9 and can be found at https://github.com/meyer-lab/systemsSerology.  We have provided a "Data Availability" section at the end of our paper. We will also generate a Digital Object Identifier (DOI) for our code once the code is finalized for the paper. </t>
   </si>
 </sst>
 </file>
@@ -1122,57 +1149,6 @@
     <xf numFmtId="0" fontId="25" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="23" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="25" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="26" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
@@ -1181,22 +1157,16 @@
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
     <xf numFmtId="0" fontId="11" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1"/>
@@ -1204,6 +1174,63 @@
     <xf numFmtId="0" fontId="26" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="top" wrapText="1"/>
       <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="28" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1"/>
+    <xf numFmtId="0" fontId="7" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="14" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="29" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="30" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="32" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="33" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1550,8 +1577,8 @@
   </sheetPr>
   <dimension ref="A1:Q93"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
-      <selection activeCell="E83" sqref="E83:F83"/>
+    <sheetView tabSelected="1" topLeftCell="B79" zoomScale="110" zoomScaleNormal="75" zoomScalePageLayoutView="75" workbookViewId="0">
+      <selection activeCell="E85" sqref="E85:F85"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="21" x14ac:dyDescent="0.25"/>
@@ -1572,60 +1599,60 @@
       <c r="E1" s="6"/>
     </row>
     <row r="2" spans="2:7" ht="37" x14ac:dyDescent="0.45">
-      <c r="B2" s="35" t="s">
+      <c r="B2" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="36"/>
-      <c r="D2" s="36"/>
+      <c r="C2" s="58"/>
+      <c r="D2" s="58"/>
       <c r="E2" s="6"/>
     </row>
     <row r="4" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B4" s="59" t="s">
+      <c r="B4" s="63" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="60"/>
-      <c r="D4" s="60"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
       <c r="E4" s="22"/>
       <c r="F4" s="26" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="5" spans="2:7" ht="34" x14ac:dyDescent="0.4">
-      <c r="B5" s="41" t="s">
+      <c r="B5" s="59" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
+      <c r="C5" s="60"/>
+      <c r="D5" s="60"/>
       <c r="E5" s="22"/>
       <c r="F5" s="26"/>
     </row>
     <row r="6" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="7" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B7" s="43" t="s">
-        <v>108</v>
-      </c>
-      <c r="C7" s="44"/>
-      <c r="D7" s="45"/>
+      <c r="B7" s="40" t="s">
+        <v>107</v>
+      </c>
+      <c r="C7" s="61"/>
+      <c r="D7" s="62"/>
       <c r="E7" s="23"/>
       <c r="F7" s="33"/>
       <c r="G7" s="34"/>
     </row>
     <row r="8" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B8" s="43" t="s">
-        <v>109</v>
-      </c>
-      <c r="C8" s="44"/>
-      <c r="D8" s="45"/>
+      <c r="B8" s="40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C8" s="61"/>
+      <c r="D8" s="62"/>
       <c r="E8" s="23"/>
       <c r="F8" s="33"/>
       <c r="G8" s="34"/>
     </row>
     <row r="9" spans="2:7" ht="27" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B9" s="43" t="s">
-        <v>110</v>
-      </c>
-      <c r="C9" s="62"/>
-      <c r="D9" s="63"/>
+      <c r="B9" s="40" t="s">
+        <v>113</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="42"/>
       <c r="E9" s="23"/>
       <c r="F9" s="28" t="s">
         <v>41</v>
@@ -1643,11 +1670,11 @@
       </c>
     </row>
     <row r="11" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="44" t="s">
         <v>106</v>
       </c>
-      <c r="C11" s="37"/>
-      <c r="D11" s="38"/>
+      <c r="C11" s="44"/>
+      <c r="D11" s="45"/>
       <c r="E11" s="17"/>
       <c r="F11" s="28" t="s">
         <v>39</v>
@@ -1657,11 +1684,11 @@
       </c>
     </row>
     <row r="12" spans="2:7" ht="76" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B12" s="39" t="s">
+      <c r="B12" s="52" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="39"/>
-      <c r="D12" s="40"/>
+      <c r="C12" s="52"/>
+      <c r="D12" s="53"/>
       <c r="E12" s="18"/>
       <c r="F12" s="28" t="s">
         <v>46</v>
@@ -1679,11 +1706,11 @@
       </c>
     </row>
     <row r="14" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B14" s="37" t="s">
+      <c r="B14" s="44" t="s">
         <v>78</v>
       </c>
-      <c r="C14" s="37"/>
-      <c r="D14" s="38"/>
+      <c r="C14" s="44"/>
+      <c r="D14" s="45"/>
       <c r="E14" s="17"/>
       <c r="F14" s="29" t="s">
         <v>50</v>
@@ -1693,11 +1720,11 @@
       </c>
     </row>
     <row r="15" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B15" s="37" t="s">
+      <c r="B15" s="44" t="s">
         <v>79</v>
       </c>
-      <c r="C15" s="37"/>
-      <c r="D15" s="38"/>
+      <c r="C15" s="44"/>
+      <c r="D15" s="45"/>
       <c r="E15" s="17"/>
       <c r="F15" s="29" t="s">
         <v>52</v>
@@ -1707,11 +1734,11 @@
       </c>
     </row>
     <row r="16" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B16" s="37" t="s">
+      <c r="B16" s="44" t="s">
         <v>80</v>
       </c>
-      <c r="C16" s="37"/>
-      <c r="D16" s="38"/>
+      <c r="C16" s="44"/>
+      <c r="D16" s="45"/>
       <c r="E16" s="17"/>
       <c r="F16" s="29" t="s">
         <v>54</v>
@@ -1724,10 +1751,10 @@
       <c r="B17" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C17" s="48" t="s">
+      <c r="C17" s="46" t="s">
         <v>82</v>
       </c>
-      <c r="D17" s="55"/>
+      <c r="D17" s="47"/>
       <c r="E17" s="24"/>
       <c r="F17" s="29" t="s">
         <v>56</v>
@@ -1740,10 +1767,10 @@
       <c r="B18" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="48" t="s">
+      <c r="C18" s="46" t="s">
         <v>81</v>
       </c>
-      <c r="D18" s="55"/>
+      <c r="D18" s="47"/>
       <c r="E18" s="24"/>
       <c r="F18" s="28" t="s">
         <v>58</v>
@@ -1756,10 +1783,10 @@
       <c r="B19" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C19" s="48" t="s">
+      <c r="C19" s="46" t="s">
         <v>9</v>
       </c>
-      <c r="D19" s="55"/>
+      <c r="D19" s="47"/>
       <c r="E19" s="24"/>
       <c r="F19" s="28" t="s">
         <v>61</v>
@@ -1772,10 +1799,10 @@
       <c r="B20" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C20" s="48" t="s">
+      <c r="C20" s="46" t="s">
         <v>10</v>
       </c>
-      <c r="D20" s="55"/>
+      <c r="D20" s="47"/>
       <c r="E20" s="24"/>
       <c r="F20" s="28" t="s">
         <v>12</v>
@@ -1788,10 +1815,10 @@
       <c r="B21" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C21" s="48" t="s">
+      <c r="C21" s="46" t="s">
         <v>2</v>
       </c>
-      <c r="D21" s="55"/>
+      <c r="D21" s="47"/>
       <c r="E21" s="24"/>
       <c r="F21" s="28" t="s">
         <v>14</v>
@@ -1808,11 +1835,11 @@
     </row>
     <row r="23" spans="1:17" s="2" customFormat="1" ht="26" x14ac:dyDescent="0.3">
       <c r="A23" s="9"/>
-      <c r="B23" s="37" t="s">
+      <c r="B23" s="44" t="s">
         <v>83</v>
       </c>
-      <c r="C23" s="37"/>
-      <c r="D23" s="38"/>
+      <c r="C23" s="44"/>
+      <c r="D23" s="45"/>
       <c r="E23" s="17"/>
       <c r="F23" s="28" t="s">
         <v>18</v>
@@ -1833,11 +1860,11 @@
     </row>
     <row r="24" spans="1:17" s="2" customFormat="1" ht="51" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A24" s="9"/>
-      <c r="B24" s="37" t="s">
+      <c r="B24" s="44" t="s">
         <v>84</v>
       </c>
-      <c r="C24" s="37"/>
-      <c r="D24" s="56"/>
+      <c r="C24" s="44"/>
+      <c r="D24" s="49"/>
       <c r="E24" s="19"/>
       <c r="F24" s="28" t="s">
         <v>16</v>
@@ -1860,10 +1887,10 @@
       <c r="B25" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C25" s="48" t="s">
+      <c r="C25" s="46" t="s">
         <v>85</v>
       </c>
-      <c r="D25" s="49"/>
+      <c r="D25" s="48"/>
       <c r="E25" s="25"/>
       <c r="F25" s="28" t="s">
         <v>25</v>
@@ -1876,10 +1903,10 @@
       <c r="B26" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C26" s="48" t="s">
+      <c r="C26" s="46" t="s">
         <v>86</v>
       </c>
-      <c r="D26" s="49"/>
+      <c r="D26" s="48"/>
       <c r="E26" s="25"/>
       <c r="F26" s="28" t="s">
         <v>21</v>
@@ -1892,10 +1919,10 @@
       <c r="B27" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C27" s="48" t="s">
+      <c r="C27" s="46" t="s">
         <v>87</v>
       </c>
-      <c r="D27" s="49"/>
+      <c r="D27" s="48"/>
       <c r="E27" s="25"/>
       <c r="F27" s="28" t="s">
         <v>23</v>
@@ -1908,50 +1935,50 @@
       <c r="B28" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C28" s="48" t="s">
+      <c r="C28" s="46" t="s">
         <v>88</v>
       </c>
-      <c r="D28" s="49"/>
+      <c r="D28" s="48"/>
       <c r="E28" s="25"/>
     </row>
     <row r="29" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B29" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C29" s="48" t="s">
+      <c r="C29" s="46" t="s">
         <v>89</v>
       </c>
-      <c r="D29" s="49"/>
+      <c r="D29" s="48"/>
       <c r="E29" s="25"/>
     </row>
     <row r="30" spans="1:17" ht="41" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C30" s="48" t="s">
+      <c r="C30" s="46" t="s">
         <v>90</v>
       </c>
-      <c r="D30" s="49"/>
+      <c r="D30" s="48"/>
       <c r="E30" s="25"/>
     </row>
     <row r="31" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B31" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C31" s="48" t="s">
+      <c r="C31" s="46" t="s">
         <v>91</v>
       </c>
-      <c r="D31" s="49"/>
+      <c r="D31" s="48"/>
       <c r="E31" s="25"/>
     </row>
     <row r="32" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B32" s="7" t="s">
         <v>95</v>
       </c>
-      <c r="C32" s="48" t="s">
+      <c r="C32" s="46" t="s">
         <v>92</v>
       </c>
-      <c r="D32" s="49"/>
+      <c r="D32" s="48"/>
       <c r="E32" s="25"/>
     </row>
     <row r="33" spans="2:7" ht="66" x14ac:dyDescent="0.25">
@@ -2021,38 +2048,38 @@
       <c r="E39" s="11"/>
     </row>
     <row r="40" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B40" s="39" t="s">
+      <c r="B40" s="52" t="s">
         <v>62</v>
       </c>
-      <c r="C40" s="39"/>
-      <c r="D40" s="40"/>
+      <c r="C40" s="52"/>
+      <c r="D40" s="53"/>
       <c r="E40" s="18"/>
     </row>
     <row r="41" spans="2:7" ht="28" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B41" s="50" t="s">
+      <c r="B41" s="54" t="s">
         <v>101</v>
       </c>
-      <c r="C41" s="50"/>
-      <c r="D41" s="51"/>
+      <c r="C41" s="54"/>
+      <c r="D41" s="55"/>
       <c r="E41" s="20"/>
     </row>
     <row r="43" spans="2:7" ht="95" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B43" s="52" t="s">
+      <c r="B43" s="56" t="s">
         <v>102</v>
       </c>
-      <c r="C43" s="52"/>
-      <c r="D43" s="52"/>
+      <c r="C43" s="56"/>
+      <c r="D43" s="56"/>
     </row>
     <row r="45" spans="2:7" ht="26" x14ac:dyDescent="0.3">
-      <c r="B45" s="46" t="s">
+      <c r="B45" s="37" t="s">
         <v>63</v>
       </c>
-      <c r="C45" s="46"/>
-      <c r="D45" s="47"/>
-      <c r="E45" s="57" t="s">
+      <c r="C45" s="37"/>
+      <c r="D45" s="38"/>
+      <c r="E45" s="50" t="s">
         <v>4</v>
       </c>
-      <c r="F45" s="58"/>
+      <c r="F45" s="51"/>
       <c r="G45" s="27"/>
     </row>
     <row r="46" spans="2:7" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2060,85 +2087,107 @@
       <c r="D47" s="12" t="s">
         <v>64</v>
       </c>
-      <c r="E47" s="61"/>
-      <c r="F47" s="54"/>
+      <c r="E47" s="39" t="s">
+        <v>119</v>
+      </c>
+      <c r="F47" s="36"/>
     </row>
     <row r="48" spans="2:7" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D48" s="12" t="s">
         <v>65</v>
       </c>
-      <c r="E48" s="61"/>
-      <c r="F48" s="54"/>
+      <c r="E48" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F48" s="36"/>
     </row>
     <row r="49" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D49" s="12" t="s">
         <v>66</v>
       </c>
-      <c r="E49" s="53"/>
-      <c r="F49" s="54"/>
+      <c r="E49" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F49" s="36"/>
     </row>
     <row r="50" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="12" t="s">
         <v>67</v>
       </c>
-      <c r="E50" s="53"/>
-      <c r="F50" s="54"/>
+      <c r="E50" s="39" t="s">
+        <v>117</v>
+      </c>
+      <c r="F50" s="36"/>
     </row>
     <row r="51" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D51" s="12" t="s">
         <v>68</v>
       </c>
-      <c r="E51" s="53"/>
-      <c r="F51" s="54"/>
+      <c r="E51" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F51" s="36"/>
     </row>
     <row r="52" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D52" s="12" t="s">
         <v>69</v>
       </c>
-      <c r="E52" s="53"/>
-      <c r="F52" s="54"/>
+      <c r="E52" s="35" t="s">
+        <v>118</v>
+      </c>
+      <c r="F52" s="36"/>
     </row>
     <row r="53" spans="2:6" ht="85" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D53" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="E53" s="53"/>
-      <c r="F53" s="54"/>
+      <c r="E53" s="35" t="s">
+        <v>117</v>
+      </c>
+      <c r="F53" s="36"/>
     </row>
     <row r="54" spans="2:6" ht="131" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D54" s="12" t="s">
         <v>71</v>
       </c>
-      <c r="E54" s="53"/>
-      <c r="F54" s="54"/>
+      <c r="E54" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F54" s="36"/>
     </row>
     <row r="55" spans="2:6" ht="156" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D55" s="12" t="s">
         <v>72</v>
       </c>
-      <c r="E55" s="53"/>
-      <c r="F55" s="54"/>
+      <c r="E55" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F55" s="36"/>
     </row>
     <row r="56" spans="2:6" ht="57" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D56" s="12" t="s">
         <v>73</v>
       </c>
-      <c r="E56" s="53"/>
-      <c r="F56" s="64"/>
+      <c r="E56" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F56" s="43"/>
     </row>
     <row r="57" spans="2:6" ht="106" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D57" s="12" t="s">
         <v>74</v>
       </c>
-      <c r="E57" s="53"/>
-      <c r="F57" s="54"/>
+      <c r="E57" s="35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F57" s="36"/>
     </row>
     <row r="59" spans="2:6" ht="26" x14ac:dyDescent="0.3">
-      <c r="B59" s="46" t="s">
+      <c r="B59" s="37" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="46"/>
-      <c r="D59" s="47"/>
+      <c r="C59" s="37"/>
+      <c r="D59" s="38"/>
       <c r="E59" s="21"/>
     </row>
     <row r="60" spans="2:6" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2146,15 +2195,19 @@
       <c r="D61" s="12" t="s">
         <v>27</v>
       </c>
-      <c r="E61" s="53"/>
-      <c r="F61" s="54"/>
+      <c r="E61" s="35" t="s">
+        <v>115</v>
+      </c>
+      <c r="F61" s="36"/>
     </row>
     <row r="62" spans="2:6" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D62" s="12" t="s">
         <v>76</v>
       </c>
-      <c r="E62" s="53"/>
-      <c r="F62" s="54"/>
+      <c r="E62" s="35" t="s">
+        <v>114</v>
+      </c>
+      <c r="F62" s="36"/>
     </row>
     <row r="63" spans="2:6" ht="22" x14ac:dyDescent="0.25">
       <c r="D63" s="13" t="s">
@@ -2169,11 +2222,11 @@
       <c r="F64" s="14"/>
     </row>
     <row r="65" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B65" s="46" t="s">
+      <c r="B65" s="37" t="s">
         <v>77</v>
       </c>
-      <c r="C65" s="46"/>
-      <c r="D65" s="47"/>
+      <c r="C65" s="37"/>
+      <c r="D65" s="38"/>
       <c r="E65" s="21"/>
     </row>
     <row r="66" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2181,41 +2234,41 @@
       <c r="D67" s="12" t="s">
         <v>30</v>
       </c>
-      <c r="E67" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F67" s="54"/>
+      <c r="E67" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F67" s="36"/>
       <c r="H67" s="16"/>
     </row>
     <row r="68" spans="2:8" ht="113" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D68" s="12" t="s">
         <v>31</v>
       </c>
-      <c r="E68" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F68" s="54"/>
+      <c r="E68" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F68" s="36"/>
       <c r="H68" s="16"/>
     </row>
     <row r="69" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D69" s="12" t="s">
         <v>3</v>
       </c>
-      <c r="E69" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F69" s="54"/>
+      <c r="E69" s="35" t="s">
+        <v>108</v>
+      </c>
+      <c r="F69" s="36"/>
       <c r="H69" s="16"/>
     </row>
     <row r="70" spans="2:8" x14ac:dyDescent="0.25">
       <c r="H70" s="16"/>
     </row>
     <row r="71" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B71" s="46" t="s">
+      <c r="B71" s="37" t="s">
         <v>32</v>
       </c>
-      <c r="C71" s="46"/>
-      <c r="D71" s="47"/>
+      <c r="C71" s="37"/>
+      <c r="D71" s="38"/>
       <c r="E71" s="21"/>
     </row>
     <row r="72" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2223,75 +2276,75 @@
       <c r="D73" s="12" t="s">
         <v>33</v>
       </c>
-      <c r="E73" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F73" s="54"/>
+      <c r="E73" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F73" s="36"/>
     </row>
     <row r="74" spans="2:8" ht="111" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D74" s="12" t="s">
         <v>34</v>
       </c>
-      <c r="E74" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F74" s="54"/>
+      <c r="E74" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F74" s="36"/>
       <c r="H74" s="16"/>
     </row>
     <row r="75" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D75" s="12" t="s">
         <v>35</v>
       </c>
-      <c r="E75" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F75" s="54"/>
+      <c r="E75" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F75" s="36"/>
       <c r="H75" s="16"/>
     </row>
     <row r="76" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D76" s="12" t="s">
         <v>36</v>
       </c>
-      <c r="E76" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F76" s="54"/>
+      <c r="E76" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F76" s="36"/>
       <c r="H76" s="16"/>
     </row>
     <row r="77" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D77" s="12" t="s">
         <v>28</v>
       </c>
-      <c r="E77" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F77" s="54"/>
+      <c r="E77" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F77" s="36"/>
       <c r="H77" s="16"/>
     </row>
     <row r="78" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D78" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E78" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F78" s="54"/>
+      <c r="E78" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F78" s="36"/>
     </row>
     <row r="79" spans="2:8" ht="71" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D79" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="E79" s="53" t="s">
-        <v>111</v>
-      </c>
-      <c r="F79" s="54"/>
+      <c r="E79" s="35" t="s">
+        <v>109</v>
+      </c>
+      <c r="F79" s="36"/>
     </row>
     <row r="81" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B81" s="46" t="s">
+      <c r="B81" s="37" t="s">
         <v>37</v>
       </c>
-      <c r="C81" s="46"/>
-      <c r="D81" s="47"/>
+      <c r="C81" s="37"/>
+      <c r="D81" s="38"/>
       <c r="E81" s="21"/>
     </row>
     <row r="82" spans="2:8" ht="22" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -2299,31 +2352,39 @@
       <c r="D83" s="12" t="s">
         <v>103</v>
       </c>
-      <c r="E83" s="53"/>
-      <c r="F83" s="54"/>
+      <c r="E83" s="35" t="s">
+        <v>120</v>
+      </c>
+      <c r="F83" s="36"/>
     </row>
     <row r="84" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D84" s="12" t="s">
         <v>29</v>
       </c>
-      <c r="E84" s="53"/>
-      <c r="F84" s="54"/>
+      <c r="E84" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F84" s="36"/>
       <c r="H84" s="16"/>
     </row>
     <row r="85" spans="2:8" ht="89" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D85" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="E85" s="53"/>
-      <c r="F85" s="54"/>
+      <c r="E85" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F85" s="36"/>
       <c r="H85" s="16"/>
     </row>
     <row r="86" spans="2:8" ht="133" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D86" s="12" t="s">
         <v>104</v>
       </c>
-      <c r="E86" s="53"/>
-      <c r="F86" s="54"/>
+      <c r="E86" s="35" t="s">
+        <v>110</v>
+      </c>
+      <c r="F86" s="36"/>
       <c r="H86" s="16"/>
     </row>
     <row r="87" spans="2:8" x14ac:dyDescent="0.25">
@@ -2332,11 +2393,11 @@
       <c r="F87" s="14"/>
     </row>
     <row r="88" spans="2:8" ht="26" x14ac:dyDescent="0.3">
-      <c r="B88" s="46" t="s">
+      <c r="B88" s="37" t="s">
         <v>38</v>
       </c>
-      <c r="C88" s="46"/>
-      <c r="D88" s="47"/>
+      <c r="C88" s="37"/>
+      <c r="D88" s="38"/>
       <c r="E88" s="21"/>
       <c r="H88" s="16"/>
     </row>
@@ -2347,10 +2408,10 @@
       <c r="D90" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="E90" s="53" t="s">
-        <v>107</v>
-      </c>
-      <c r="F90" s="54"/>
+      <c r="E90" s="35" t="s">
+        <v>111</v>
+      </c>
+      <c r="F90" s="36"/>
       <c r="H90" s="16"/>
     </row>
     <row r="91" spans="2:8" x14ac:dyDescent="0.25">
@@ -2365,23 +2426,37 @@
   </sheetData>
   <sheetProtection password="DCD2" sheet="1" objects="1" scenarios="1"/>
   <mergeCells count="64">
-    <mergeCell ref="E90:F90"/>
-    <mergeCell ref="E76:F76"/>
-    <mergeCell ref="E77:F77"/>
-    <mergeCell ref="E78:F78"/>
-    <mergeCell ref="E79:F79"/>
-    <mergeCell ref="E83:F83"/>
-    <mergeCell ref="E84:F84"/>
-    <mergeCell ref="E85:F85"/>
-    <mergeCell ref="E86:F86"/>
-    <mergeCell ref="E67:F67"/>
-    <mergeCell ref="E68:F68"/>
-    <mergeCell ref="E69:F69"/>
-    <mergeCell ref="B88:D88"/>
-    <mergeCell ref="B81:D81"/>
-    <mergeCell ref="E73:F73"/>
-    <mergeCell ref="E74:F74"/>
-    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B5:D5"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B7:D7"/>
+    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="C26:D26"/>
+    <mergeCell ref="C27:D27"/>
+    <mergeCell ref="C28:D28"/>
+    <mergeCell ref="C31:D31"/>
+    <mergeCell ref="B40:D40"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="C32:D32"/>
+    <mergeCell ref="C30:D30"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="C21:D21"/>
+    <mergeCell ref="E45:F45"/>
+    <mergeCell ref="C25:D25"/>
+    <mergeCell ref="E47:F47"/>
+    <mergeCell ref="C19:D19"/>
+    <mergeCell ref="C20:D20"/>
+    <mergeCell ref="C29:D29"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B23:D23"/>
     <mergeCell ref="E48:F48"/>
     <mergeCell ref="E49:F49"/>
     <mergeCell ref="E50:F50"/>
@@ -2398,37 +2473,23 @@
     <mergeCell ref="B15:D15"/>
     <mergeCell ref="C17:D17"/>
     <mergeCell ref="C18:D18"/>
-    <mergeCell ref="C19:D19"/>
-    <mergeCell ref="C20:D20"/>
-    <mergeCell ref="C29:D29"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="C21:D21"/>
-    <mergeCell ref="E45:F45"/>
-    <mergeCell ref="C25:D25"/>
-    <mergeCell ref="E47:F47"/>
-    <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="C26:D26"/>
-    <mergeCell ref="C27:D27"/>
-    <mergeCell ref="C28:D28"/>
-    <mergeCell ref="C31:D31"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="C32:D32"/>
-    <mergeCell ref="C30:D30"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B5:D5"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B7:D7"/>
-    <mergeCell ref="B4:D4"/>
+    <mergeCell ref="E67:F67"/>
+    <mergeCell ref="E68:F68"/>
+    <mergeCell ref="E69:F69"/>
+    <mergeCell ref="B88:D88"/>
+    <mergeCell ref="B81:D81"/>
+    <mergeCell ref="E73:F73"/>
+    <mergeCell ref="E74:F74"/>
+    <mergeCell ref="E75:F75"/>
+    <mergeCell ref="E90:F90"/>
+    <mergeCell ref="E76:F76"/>
+    <mergeCell ref="E77:F77"/>
+    <mergeCell ref="E78:F78"/>
+    <mergeCell ref="E79:F79"/>
+    <mergeCell ref="E83:F83"/>
+    <mergeCell ref="E84:F84"/>
+    <mergeCell ref="E85:F85"/>
+    <mergeCell ref="E86:F86"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
   <hyperlinks>

</xml_diff>